<commit_message>
R Scripts and Echo Protocols
</commit_message>
<xml_diff>
--- a/CornandPeaTrial_Cherrypick.xlsx
+++ b/CornandPeaTrial_Cherrypick.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d41790b40a8915ef/Desktop/Echo Conjugations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d41790b40a8915ef/Desktop/Evaluation-of-engineering-potential-in-undomesticated-microbes-with-VECTOR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="8_{EF36D204-93E4-400E-8707-90DE31EEFA02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B137F718-3053-4FF4-97C5-4A6C7302F934}"/>
+  <xr:revisionPtr revIDLastSave="192" documentId="8_{EF36D204-93E4-400E-8707-90DE31EEFA02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB688089-19FD-4BA9-B597-74982363896D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{15EED6FD-7240-4133-9136-E552FB445692}"/>
   </bookViews>
@@ -999,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FBC01FB-FBB7-4F92-A6F1-1E7F5FD4A2BF}">
   <dimension ref="A1:P1330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N96" sqref="N96"/>
+    <sheetView tabSelected="1" topLeftCell="A1317" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I1237" sqref="I1237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>